<commit_message>
Tutor add class flow
</commit_message>
<xml_diff>
--- a/TestDataXls/Tutor Add Camp.xlsx
+++ b/TestDataXls/Tutor Add Camp.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C0F5AF-A2A1-4520-AC9B-EF1DDA78B7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A98E981-7734-4B7F-9B3A-F74FE078D410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="75">
   <si>
     <t>password</t>
   </si>
@@ -164,9 +164,6 @@
     <t>D:\nurtem-test\picturesprofile1\tennis3.jpg</t>
   </si>
   <si>
-    <t>D:\nurtem-test\picturesprofile1\tennis4.jpg</t>
-  </si>
-  <si>
     <t>This is French camp teaching how the history where they conquered puducherry</t>
   </si>
   <si>
@@ -233,18 +230,9 @@
     <t>chess</t>
   </si>
   <si>
-    <t>31/05/2022</t>
-  </si>
-  <si>
-    <t>tutor39@nkt.com</t>
-  </si>
-  <si>
     <t>camp chess 5</t>
   </si>
   <si>
-    <t>18/05/2022</t>
-  </si>
-  <si>
     <t>math 1</t>
   </si>
   <si>
@@ -264,6 +252,15 @@
   </si>
   <si>
     <t>23/11/2022</t>
+  </si>
+  <si>
+    <t>tutor53@nkt.com</t>
+  </si>
+  <si>
+    <t>07/12/2022</t>
+  </si>
+  <si>
+    <t>31/01/2023</t>
   </si>
 </sst>
 </file>
@@ -683,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -804,7 +801,7 @@
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
         <v>30</v>
@@ -834,7 +831,7 @@
         <v>38</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M2" s="2">
         <v>18100</v>
@@ -843,13 +840,13 @@
         <v>1</v>
       </c>
       <c r="O2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="Q2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>27</v>
@@ -867,10 +864,10 @@
         <v>1</v>
       </c>
       <c r="W2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="X2" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="X2" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="Y2">
         <v>1</v>
@@ -884,7 +881,7 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
         <v>30</v>
@@ -899,7 +896,7 @@
         <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H3" t="s">
         <v>31</v>
@@ -914,7 +911,7 @@
         <v>39</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M3" s="2">
         <v>18100</v>
@@ -923,13 +920,13 @@
         <v>1</v>
       </c>
       <c r="O3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="Q3" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R3" s="3" t="s">
         <v>27</v>
@@ -947,10 +944,10 @@
         <v>1</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X3" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Y3">
         <v>2</v>
@@ -964,7 +961,7 @@
         <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
         <v>30</v>
@@ -979,7 +976,7 @@
         <v>36</v>
       </c>
       <c r="G4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H4" t="s">
         <v>31</v>
@@ -994,7 +991,7 @@
         <v>40</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M4" s="2">
         <v>18100</v>
@@ -1003,19 +1000,19 @@
         <v>1</v>
       </c>
       <c r="O4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="P4" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P4" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="Q4" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="S4" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="T4" s="4">
         <v>20</v>
@@ -1027,10 +1024,10 @@
         <v>1</v>
       </c>
       <c r="W4" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="X4" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Y4">
         <v>3</v>
@@ -1047,16 +1044,16 @@
         <v>30</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" t="s">
         <v>58</v>
-      </c>
-      <c r="G5" t="s">
-        <v>59</v>
       </c>
       <c r="H5" t="s">
         <v>31</v>
@@ -1071,7 +1068,7 @@
         <v>41</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M5" s="2">
         <v>18100</v>
@@ -1080,19 +1077,19 @@
         <v>1</v>
       </c>
       <c r="O5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q5" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="P5" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="R5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="S5" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="S5" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="T5" s="4">
         <v>16</v>
@@ -1104,10 +1101,10 @@
         <v>1</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="X5" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Y5">
         <v>4</v>
@@ -1121,22 +1118,22 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
         <v>30</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" t="s">
         <v>64</v>
-      </c>
-      <c r="G6" t="s">
-        <v>67</v>
       </c>
       <c r="H6" t="s">
         <v>31</v>
@@ -1148,10 +1145,10 @@
         <v>20</v>
       </c>
       <c r="K6" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M6" s="2">
         <v>18100</v>
@@ -1160,19 +1157,19 @@
         <v>1</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="R6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="S6" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="T6" s="4">
         <v>16</v>
@@ -1184,10 +1181,10 @@
         <v>1</v>
       </c>
       <c r="W6" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="X6" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Y6">
         <v>5</v>
@@ -1201,22 +1198,22 @@
         <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H7" t="s">
         <v>31</v>
@@ -1228,10 +1225,10 @@
         <v>20</v>
       </c>
       <c r="K7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M7" s="2">
         <v>18100</v>
@@ -1240,19 +1237,19 @@
         <v>1</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="R7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="S7" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="S7" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="T7" s="4">
         <v>16</v>
@@ -1264,10 +1261,10 @@
         <v>1</v>
       </c>
       <c r="W7" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="X7" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Y7">
         <v>5</v>

</xml_diff>